<commit_message>
Update of contribution_empirical; addition of a third scenario, accounting for retention of nutrients from the digestible fraction
</commit_message>
<xml_diff>
--- a/data/solubility/Aquaponics - Masterfile Nutrients.xlsx
+++ b/data/solubility/Aquaponics - Masterfile Nutrients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anilaxeltellbuescher/Projekte/Projekt18 - PhD-Aquaponics/data/solubility/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD/Projekte/Projekt18 - PhD-Aquaponics/data/solubility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB1D3F5-9C86-5946-BC93-1A4355254541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD41A2B9-6646-F44A-90B0-485A9E3B47B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="956" firstSheet="7" activeTab="16" xr2:uid="{5855CA20-A45B-EF4D-A216-6F07AE6CF6F3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="33600" tabRatio="956" firstSheet="1" activeTab="7" xr2:uid="{5855CA20-A45B-EF4D-A216-6F07AE6CF6F3}"/>
   </bookViews>
   <sheets>
     <sheet name="important notes" sheetId="1" r:id="rId1"/>
@@ -13581,9 +13581,6 @@
     <t>country</t>
   </si>
   <si>
-    <t>ec_µScm</t>
-  </si>
-  <si>
     <t>NH4_mgL</t>
   </si>
   <si>
@@ -13597,9 +13594,6 @@
   </si>
   <si>
     <t>SO4-S_mgL</t>
-  </si>
-  <si>
-    <t>Zn_µgL</t>
   </si>
   <si>
     <t>Cl_mgL</t>
@@ -13764,6 +13758,12 @@
   </si>
   <si>
     <t>Auburn</t>
+  </si>
+  <si>
+    <t>Zn_ugL</t>
+  </si>
+  <si>
+    <t>ec_uScm</t>
   </si>
 </sst>
 </file>
@@ -14224,7 +14224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -14325,6 +14325,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -14337,9 +14339,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -14367,16 +14366,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -14392,6 +14381,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -17194,7 +17193,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{713B421E-3016-4993-8813-5FAFECEBF423}" name="Table1" displayName="Table1" ref="A1:BE48" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{713B421E-3016-4993-8813-5FAFECEBF423}" name="Table1" displayName="Table1" ref="A1:BE48" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:BE48" xr:uid="{713B421E-3016-4993-8813-5FAFECEBF423}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BE47">
     <sortCondition ref="A1:A47"/>
@@ -17295,7 +17294,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-Design 2013–2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -17583,7 +17582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -17648,12 +17647,12 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
@@ -17663,7 +17662,7 @@
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
@@ -17730,7 +17729,7 @@
   <sheetData>
     <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>feedIN!F2</f>
@@ -17871,7 +17870,7 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B2">
         <f>COUNT(feedIN!F3:F196)</f>
@@ -18012,7 +18011,7 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B3" s="4">
         <f>MIN(feedIN!F3:F196)</f>
@@ -18153,7 +18152,7 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B4" s="4">
         <f>AVERAGE(feedIN!F3:F196)</f>
@@ -18435,7 +18434,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B6" s="4">
         <f>MAX(feedIN!F3:F196)</f>
@@ -18576,7 +18575,7 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E7">
         <f>1000*E3/6.25</f>
@@ -18585,7 +18584,7 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E8">
         <f>1000*E4/6.25</f>
@@ -18594,7 +18593,7 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E9">
         <f>1000*E5/6.25</f>
@@ -18603,7 +18602,7 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E10">
         <f>1000*E6/6.25</f>
@@ -18644,12 +18643,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="99" t="s">
         <v>406</v>
       </c>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="98"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="100"/>
     </row>
     <row r="2" spans="1:41" s="25" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="str">
@@ -22418,22 +22417,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="24" x14ac:dyDescent="0.3">
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96"/>
-      <c r="V1" s="96" t="s">
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
-      <c r="Y1" s="96"/>
-      <c r="Z1" s="96"/>
-      <c r="AA1" s="96"/>
-      <c r="AB1" s="96"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98"/>
     </row>
     <row r="2" spans="1:29" s="25" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -35072,22 +35071,22 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96" t="s">
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
-      <c r="Y1" s="96"/>
-      <c r="Z1" s="96"/>
-      <c r="AA1" s="96"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
       <c r="AB1" s="7"/>
     </row>
     <row r="2" spans="1:28" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -36791,8 +36790,8 @@
   </sheetPr>
   <dimension ref="A1:Y116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D102" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="F70" sqref="F70"/>
@@ -36813,30 +36812,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="24" x14ac:dyDescent="0.3">
-      <c r="G1" s="96" t="s">
+      <c r="G1" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96" t="s">
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96"/>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -37218,7 +37217,7 @@
         <f>rearing!C21</f>
         <v>RAS A</v>
       </c>
-      <c r="E21" s="102">
+      <c r="E21" s="97">
         <f>324.6/rearing!N21*1000</f>
         <v>329.93721973094171</v>
       </c>
@@ -37236,7 +37235,7 @@
         <f>rearing!C22</f>
         <v>RAS C+Hydro C</v>
       </c>
-      <c r="E22" s="102">
+      <c r="E22" s="97">
         <f>330.2/rearing!N22*1000</f>
         <v>336.1317365269461</v>
       </c>
@@ -37254,7 +37253,7 @@
         <f>rearing!C23</f>
         <v>RAS D/Hydro D</v>
       </c>
-      <c r="E23" s="102">
+      <c r="E23" s="97">
         <f>323.7/rearing!N23*1000</f>
         <v>329.51497005988028</v>
       </c>
@@ -38876,27 +38875,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="24" x14ac:dyDescent="0.3">
-      <c r="Y1" s="99"/>
-      <c r="Z1" s="99"/>
-      <c r="AA1" s="99"/>
-      <c r="AB1" s="99"/>
-      <c r="AC1" s="99"/>
-      <c r="AD1" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE1" s="99"/>
-      <c r="AF1" s="99"/>
-      <c r="AG1" s="99"/>
-      <c r="AH1" s="99"/>
-      <c r="AI1" s="99" t="s">
+      <c r="Y1" s="101"/>
+      <c r="Z1" s="101"/>
+      <c r="AA1" s="101"/>
+      <c r="AB1" s="101"/>
+      <c r="AC1" s="101"/>
+      <c r="AD1" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE1" s="101"/>
+      <c r="AF1" s="101"/>
+      <c r="AG1" s="101"/>
+      <c r="AH1" s="101"/>
+      <c r="AI1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="AJ1" s="99"/>
-      <c r="AK1" s="99"/>
-      <c r="AL1" s="99"/>
-      <c r="AM1" s="99"/>
-      <c r="AN1" s="99"/>
-      <c r="AO1" s="99"/>
+      <c r="AJ1" s="101"/>
+      <c r="AK1" s="101"/>
+      <c r="AL1" s="101"/>
+      <c r="AM1" s="101"/>
+      <c r="AN1" s="101"/>
+      <c r="AO1" s="101"/>
     </row>
     <row r="2" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -46356,7 +46355,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:E236">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46794,7 +46793,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="64" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C6" s="64">
         <v>4</v>
@@ -48056,7 +48055,7 @@
         <v>1</v>
       </c>
       <c r="O40" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -48064,13 +48063,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C41">
         <v>4</v>
       </c>
       <c r="O41" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -48087,8 +48086,8 @@
   <dimension ref="A1:N206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J120" sqref="J120"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F106" sqref="F102:F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -58012,7 +58011,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>160</v>
@@ -58080,7 +58079,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>160</v>
@@ -58148,7 +58147,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>160</v>
@@ -58216,7 +58215,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>160</v>
@@ -58445,11 +58444,11 @@
       <c r="M21" s="7">
         <v>4</v>
       </c>
-      <c r="N21" s="101">
+      <c r="N21" s="96">
         <f>O21/(G21/1000)</f>
         <v>983.82352941176475</v>
       </c>
-      <c r="O21" s="100">
+      <c r="O21" s="7">
         <v>66.900000000000006</v>
       </c>
       <c r="R21" s="10">
@@ -58506,11 +58505,11 @@
       <c r="M22" s="7">
         <v>4</v>
       </c>
-      <c r="N22" s="101">
-        <f t="shared" ref="N22:N23" si="3">O22/(G22/1000)</f>
+      <c r="N22" s="96">
+        <f t="shared" ref="N22" si="3">O22/(G22/1000)</f>
         <v>982.35294117647049</v>
       </c>
-      <c r="O22" s="100">
+      <c r="O22" s="7">
         <v>66.8</v>
       </c>
       <c r="R22" s="10">
@@ -58567,11 +58566,11 @@
       <c r="M23" s="7">
         <v>4</v>
       </c>
-      <c r="N23" s="101">
+      <c r="N23" s="96">
         <f>O23/(G23/1000)</f>
         <v>982.35294117647049</v>
       </c>
-      <c r="O23" s="100">
+      <c r="O23" s="7">
         <v>66.8</v>
       </c>
       <c r="R23" s="10">
@@ -60900,7 +60899,7 @@
         <v>8119.8</v>
       </c>
       <c r="P68" s="12">
-        <f t="shared" ref="P68:P69" si="16">L68*R68</f>
+        <f t="shared" ref="P68" si="16">L68*R68</f>
         <v>2.145</v>
       </c>
       <c r="Q68" s="7">
@@ -61007,7 +61006,7 @@
       <c r="L70" s="7">
         <v>3.81</v>
       </c>
-      <c r="M70" s="100">
+      <c r="M70" s="7">
         <v>1.6</v>
       </c>
       <c r="N70" s="7">
@@ -61071,7 +61070,7 @@
       <c r="L71" s="7">
         <v>3.81</v>
       </c>
-      <c r="M71" s="100">
+      <c r="M71" s="7">
         <v>1.6</v>
       </c>
       <c r="N71" s="7">
@@ -61135,7 +61134,7 @@
       <c r="L72" s="7">
         <v>3.81</v>
       </c>
-      <c r="M72" s="100">
+      <c r="M72" s="7">
         <v>1.6</v>
       </c>
       <c r="N72" s="7">
@@ -61199,7 +61198,7 @@
       <c r="L73" s="7">
         <v>3.81</v>
       </c>
-      <c r="M73" s="100">
+      <c r="M73" s="7">
         <v>1.6</v>
       </c>
       <c r="N73" s="7">
@@ -61525,7 +61524,7 @@
         <v>376</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.2">
@@ -61539,7 +61538,7 @@
         <v>368</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.2">
@@ -61553,7 +61552,7 @@
         <v>369</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.2">
@@ -61567,7 +61566,7 @@
         <v>370</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
@@ -61581,7 +61580,7 @@
         <v>371</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
@@ -61595,7 +61594,7 @@
         <v>372</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.2">
@@ -61609,7 +61608,7 @@
         <v>373</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.2">
@@ -61623,7 +61622,7 @@
         <v>374</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.2">
@@ -61637,7 +61636,7 @@
         <v>375</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.2">
@@ -62216,7 +62215,7 @@
         <v>439</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F109" s="7" t="s">
         <v>71</v>
@@ -62251,7 +62250,7 @@
         <v>440</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F110" s="7" t="s">
         <v>71</v>
@@ -62271,7 +62270,7 @@
         <v>441</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F111" s="7" t="s">
         <v>71</v>
@@ -62291,7 +62290,7 @@
         <v>442</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F112" s="7" t="s">
         <v>71</v>
@@ -62445,7 +62444,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>rearing!G2</f>
@@ -62510,7 +62509,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B2">
         <f>AVERAGE(rearing!G3:G196)</f>
@@ -62585,11 +62584,11 @@
   </sheetPr>
   <dimension ref="A1:AA117"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="N104" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q131" sqref="Q131"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -62608,29 +62607,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="J1" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96" t="s">
+      <c r="J1" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96"/>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
-      <c r="Y1" s="96" t="s">
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="96"/>
+      <c r="Z1" s="98"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -62661,19 +62660,19 @@
         <v>46</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>562</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>566</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>483</v>
@@ -62685,13 +62684,13 @@
         <v>485</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="R2" s="14" t="s">
         <v>488</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>568</v>
+        <v>614</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>490</v>
@@ -62712,7 +62711,7 @@
         <v>494</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -67140,38 +67139,38 @@
   <sheetData>
     <row r="1" spans="1:39" ht="24" x14ac:dyDescent="0.3">
       <c r="F1" s="7"/>
-      <c r="H1" s="96" t="s">
+      <c r="H1" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
       <c r="N1" s="65"/>
       <c r="O1" s="65"/>
-      <c r="P1" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="96"/>
-      <c r="U1" s="96" t="s">
+      <c r="P1" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="96"/>
-      <c r="W1" s="96"/>
-      <c r="X1" s="96"/>
-      <c r="Y1" s="96"/>
-      <c r="Z1" s="96"/>
-      <c r="AA1" s="96"/>
-      <c r="AB1" s="96" t="s">
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="AC1" s="96"/>
-      <c r="AD1" s="96"/>
-      <c r="AE1" s="96"/>
+      <c r="AC1" s="98"/>
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
     </row>
     <row r="2" spans="1:39" s="25" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -67186,85 +67185,85 @@
         <v>Treatment_ID</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>569</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>570</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="G2" s="36" t="s">
         <v>571</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="H2" s="24" t="s">
         <v>572</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="I2" s="22" t="s">
         <v>573</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="J2" s="22" t="s">
         <v>574</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>575</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="L2" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="M2" s="23" t="s">
         <v>577</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="N2" s="58" t="s">
         <v>578</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="O2" s="58" t="s">
         <v>579</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="P2" s="24" t="s">
         <v>580</v>
       </c>
-      <c r="O2" s="58" t="s">
+      <c r="Q2" s="22" t="s">
         <v>581</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="R2" s="22" t="s">
         <v>582</v>
       </c>
-      <c r="Q2" s="22" t="s">
+      <c r="S2" s="22" t="s">
         <v>583</v>
       </c>
-      <c r="R2" s="22" t="s">
+      <c r="T2" s="23" t="s">
         <v>584</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="U2" s="24" t="s">
         <v>585</v>
       </c>
-      <c r="T2" s="23" t="s">
+      <c r="V2" s="22" t="s">
         <v>586</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="W2" s="22" t="s">
         <v>587</v>
       </c>
-      <c r="V2" s="22" t="s">
+      <c r="X2" s="22" t="s">
         <v>588</v>
       </c>
-      <c r="W2" s="22" t="s">
+      <c r="Y2" s="22" t="s">
         <v>589</v>
       </c>
-      <c r="X2" s="22" t="s">
+      <c r="Z2" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="Y2" s="22" t="s">
+      <c r="AA2" s="23" t="s">
         <v>591</v>
       </c>
-      <c r="Z2" s="22" t="s">
+      <c r="AB2" s="24" t="s">
         <v>592</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AC2" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="AB2" s="24" t="s">
+      <c r="AD2" s="22" t="s">
         <v>594</v>
-      </c>
-      <c r="AC2" s="22" t="s">
-        <v>595</v>
-      </c>
-      <c r="AD2" s="22" t="s">
-        <v>596</v>
       </c>
       <c r="AE2" s="22" t="s">
         <v>419</v>

</xml_diff>